<commit_message>
Codebase should now work with command prompt starts
</commit_message>
<xml_diff>
--- a/data/2/20230603-a1r-yc-session2-o_transcript.xlsx
+++ b/data/2/20230603-a1r-yc-session2-o_transcript.xlsx
@@ -1,192 +1,43 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marlibosler/Desktop/Session 2/EXCEL 06:03 session 2/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDBB45EC-B620-D441-8154-AF2B48E8CB3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="15960" windowHeight="16420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="500" windowWidth="15960" windowHeight="16420" tabRatio="600" firstSheet="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1 - 20230603-a1r-yc-sessi" sheetId="1" r:id="rId1"/>
-    <sheet name="proposal" sheetId="2" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="in" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="46">
-  <si>
-    <t>time</t>
-  </si>
-  <si>
-    <t>"19:49"</t>
-  </si>
-  <si>
-    <t>I don't know what's going on with the technology here, but I guess my comment on this would be in general. The Electoral College is fine and my opinion. I don't know all the specifics but I think it's more of the gerrymandering that happens and all the issues of that we talked about before.</t>
-  </si>
-  <si>
-    <t>"20:09"</t>
-  </si>
-  <si>
-    <t>Yes, I believe the Electoral College is fine. It gives smaller States chance and I think the reason this is up for discussion is because of the last election were the popular vote, did not reflect the Electoral College vote and it didn't either in 2000.</t>
-  </si>
-  <si>
-    <t>"20:31"</t>
-  </si>
-  <si>
-    <t>Yeah, I also agree that skipping Electoral College seems to be a good thing. I think it makes the candidates kind of a make their views known to more of the state's. The thing that I've be afraid of with the national popular vote is that it would only they would only cater to large cities and areas as opposed to the entire country.</t>
-  </si>
-  <si>
-    <t>"21:00"</t>
-  </si>
-  <si>
-    <t>Yes, none of the candidates visit California, or, you know, campaign in New York because those states are already wrapped up. So that's kind of the unfair part about it, but it seems to work.</t>
-  </si>
-  <si>
-    <t>"22:45"</t>
-  </si>
-  <si>
-    <t>Yes, this could be unconstitutional and generally, it works generally the popular vote of each state reflects the, their Electoral College votes.</t>
-  </si>
-  <si>
-    <t>"22:57"</t>
-  </si>
-  <si>
-    <t>Yeah, I also agree this. I believe this is covered in the Constitution. I don't like the idea of just kind of making this up if you were to go this way. I prefer that the Constitution be amended but I think, like we previously discussed I feel like a few of us agree that the Electoral College is working and this would kind of take that away.</t>
-  </si>
-  <si>
-    <t>"24:56"</t>
-  </si>
-  <si>
-    <t>I'm not sure sure about the limitations but I think my issue with Supreme Court has more about their heavy political affiliations when that kind of to me seems to go beyond the scope of what the intent of the position is.</t>
-  </si>
-  <si>
-    <t>"25:17"</t>
-  </si>
-  <si>
-    <t>Yeah, I feel I would actually like to see the 18-year term limits. I think when the lifetime limits were put in place way back in the 1800's life expectancy wasn't expected to be into the 80s and 90s like today and I don't really like the idea of having someone on the Supreme Court for 30 40, even 50 years, I also think would maybe take a little bit of the polarization out of it. If each president were to get to, you wouldn't have some of the games that are being played right now and it's kind of morbid. It feels like they're making current Supreme.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Or justices feel like they have to retire because they might die before a term ends, or after a term beds. So, I think this would kind of even things out a little bit better.</t>
-  </si>
-  <si>
-    <t>"26:04"</t>
-  </si>
-  <si>
-    <t>Why do we the founding fathers? Set it up. So these judges have tenure and they're Untouchable that have to worry about that and ethical decisions of the Supreme Court Justices. I think that self-regulating. I mean, we trust him enough to not do any unethical things. Obviously, that's coming up with Justice Thomas right now and giving each president,</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> it's, you know, just</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> the reason we're talking about this is because Trump was able to not put in three Supreme Court Justices, that's why this issues coming up and trying to</t>
-  </si>
-  <si>
-    <t>"28:40"</t>
-  </si>
-  <si>
-    <t>Yes, I'll be for increasing federal spending on our public schools for how our government works. I'm working with a 19 year old man right now out of high school. Who does not know? There are three branches of government. So yeah, we can do more of that.</t>
-  </si>
-  <si>
-    <t>"29:05"</t>
-  </si>
-  <si>
-    <t>Yeah, I completely agree. I think it's not a bad thing as a father to two teenagers right now. I'm not expecting like Leaps and Bounds changes. I think it's things like financial literacy in. This is kind of a higher level topic for kids, but just to give them kind of that background and so that they can kind of have those basic understandings is never a bad thing. And I think we do a better job of just giving the kids, some type of introduction to government things like financial literacy, and things like that. Just so that they have kind of an idea of what it's all about.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Out.</t>
-  </si>
-  <si>
-    <t>"33:27"</t>
-  </si>
-  <si>
-    <t>Germany is so real and it is fixed system. Maybe we could have it done by just geographical landmarks, instead like rivers and county lines instead of having. Just one street, the one district and another, the same exact story could be in another District. It's so weighted against the party in charge when they figure out.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Out these lines.</t>
-  </si>
-  <si>
-    <t>speaker</t>
-  </si>
-  <si>
-    <t>text</t>
-  </si>
-  <si>
-    <t>proposal</t>
-  </si>
-  <si>
-    <t>Implement RCV as an alternative method both to elected officials and representatives at all levels</t>
-  </si>
-  <si>
-    <t>Change the primary system</t>
-  </si>
-  <si>
-    <t>Use proportional representatives to elect elected officials</t>
-  </si>
-  <si>
-    <t>Change the current electoral college</t>
-  </si>
-  <si>
-    <t>Implement more accessibility to voting</t>
-  </si>
-  <si>
-    <t>Restore federal and state voting rights to citizens with felony convictions upon their release from prison</t>
-  </si>
-  <si>
-    <t>Implement voting standards that are less strict</t>
-  </si>
-  <si>
-    <t>Implement more measures to address voter fraud</t>
-  </si>
-  <si>
-    <t>Implement more fairness and transparency in the election process</t>
-  </si>
-  <si>
-    <t>Implement limits on financing individual candidates and parties</t>
-  </si>
-  <si>
-    <t>Increase in public funding and financing for campaigns</t>
-  </si>
-  <si>
-    <t>Implement a term limit for Supreme Court Justices</t>
-  </si>
-  <si>
-    <t>Increase opportunities for learning about civic education in schools</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="3">
     <font>
+      <name val="Helvetica Neue"/>
+      <color indexed="8"/>
       <sz val="10"/>
-      <color indexed="8"/>
-      <name val="Helvetica Neue"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color indexed="8"/>
       <name val="Arial"/>
       <family val="2"/>
+      <color indexed="8"/>
+      <sz val="10"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color indexed="8"/>
+      <sz val="11"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -262,44 +113,44 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+  <cellXfs count="10">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -368,14 +219,6 @@
       <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -1450,330 +1293,329 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:IS20"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="6.1640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="7" style="1" customWidth="1"/>
-    <col min="3" max="3" width="166.6640625" style="1" customWidth="1"/>
-    <col min="4" max="253" width="8.33203125" style="1" customWidth="1"/>
+    <col width="6.1640625" customWidth="1" style="1" min="1" max="1"/>
+    <col width="7" customWidth="1" style="1" min="2" max="2"/>
+    <col width="166.6640625" customWidth="1" style="1" min="3" max="3"/>
+    <col width="8.33203125" customWidth="1" style="1" min="4" max="253"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="4">
+    <row r="1" ht="20.25" customHeight="1" s="9">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>speaker</t>
+        </is>
+      </c>
+      <c r="B1" s="3" t="inlineStr">
+        <is>
+          <t>time</t>
+        </is>
+      </c>
+      <c r="C1" s="3" t="inlineStr">
+        <is>
+          <t>text</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="20" customHeight="1" s="9">
+      <c r="A2" s="4" t="n">
         <v>48339</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="4">
+      <c r="B2" s="5" t="inlineStr">
+        <is>
+          <t>"19:49"</t>
+        </is>
+      </c>
+      <c r="C2" s="5" t="inlineStr">
+        <is>
+          <t>I don't know what's going on with the technology here, but I guess my comment on this would be in general. The Electoral College is fine and my opinion. I don't know all the specifics but I think it's more of the gerrymandering that happens and all the issues of that we talked about before.</t>
+        </is>
+      </c>
+    </row>
+    <row r="3" ht="20" customHeight="1" s="9">
+      <c r="A3" s="4" t="n">
         <v>48508</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="4">
+      <c r="B3" s="5" t="inlineStr">
+        <is>
+          <t>"20:09"</t>
+        </is>
+      </c>
+      <c r="C3" s="5" t="inlineStr">
+        <is>
+          <t>Yes, I believe the Electoral College is fine. It gives smaller States chance and I think the reason this is up for discussion is because of the last election were the popular vote, did not reflect the Electoral College vote and it didn't either in 2000.</t>
+        </is>
+      </c>
+    </row>
+    <row r="4" ht="20" customHeight="1" s="9">
+      <c r="A4" s="4" t="n">
         <v>48470</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="6"/>
-    </row>
-    <row r="5" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="4">
+      <c r="B4" s="5" t="inlineStr">
+        <is>
+          <t>"20:31"</t>
+        </is>
+      </c>
+      <c r="C4" s="6" t="n"/>
+    </row>
+    <row r="5" ht="20" customHeight="1" s="9">
+      <c r="A5" s="4" t="n">
         <v>48470</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="4">
+      <c r="B5" s="5" t="inlineStr">
+        <is>
+          <t>"20:31"</t>
+        </is>
+      </c>
+      <c r="C5" s="5" t="inlineStr">
+        <is>
+          <t>Yeah, I also agree that skipping Electoral College seems to be a good thing. I think it makes the candidates kind of a make their views known to more of the state's. The thing that I've be afraid of with the national popular vote is that it would only they would only cater to large cities and areas as opposed to the entire country.</t>
+        </is>
+      </c>
+    </row>
+    <row r="6" ht="20" customHeight="1" s="9">
+      <c r="A6" s="4" t="n">
         <v>48508</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="4">
+      <c r="B6" s="5" t="inlineStr">
+        <is>
+          <t>"21:00"</t>
+        </is>
+      </c>
+      <c r="C6" s="5" t="inlineStr">
+        <is>
+          <t>Yes, none of the candidates visit California, or, you know, campaign in New York because those states are already wrapped up. So that's kind of the unfair part about it, but it seems to work.</t>
+        </is>
+      </c>
+    </row>
+    <row r="7" ht="20" customHeight="1" s="9">
+      <c r="A7" s="4" t="n">
         <v>48508</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="4">
+      <c r="B7" s="5" t="inlineStr">
+        <is>
+          <t>"22:45"</t>
+        </is>
+      </c>
+      <c r="C7" s="5" t="inlineStr">
+        <is>
+          <t>Yes, this could be unconstitutional and generally, it works generally the popular vote of each state reflects the, their Electoral College votes.</t>
+        </is>
+      </c>
+    </row>
+    <row r="8" ht="20" customHeight="1" s="9">
+      <c r="A8" s="4" t="n">
         <v>48470</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="4">
+      <c r="B8" s="5" t="inlineStr">
+        <is>
+          <t>"22:57"</t>
+        </is>
+      </c>
+      <c r="C8" s="5" t="inlineStr">
+        <is>
+          <t>Yeah, I also agree this. I believe this is covered in the Constitution. I don't like the idea of just kind of making this up if you were to go this way. I prefer that the Constitution be amended but I think, like we previously discussed I feel like a few of us agree that the Electoral College is working and this would kind of take that away.</t>
+        </is>
+      </c>
+    </row>
+    <row r="9" ht="20" customHeight="1" s="9">
+      <c r="A9" s="4" t="n">
         <v>48339</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="4">
+      <c r="B9" s="5" t="inlineStr">
+        <is>
+          <t>"24:56"</t>
+        </is>
+      </c>
+      <c r="C9" s="5" t="inlineStr">
+        <is>
+          <t>I'm not sure sure about the limitations but I think my issue with Supreme Court has more about their heavy political affiliations when that kind of to me seems to go beyond the scope of what the intent of the position is.</t>
+        </is>
+      </c>
+    </row>
+    <row r="10" ht="20" customHeight="1" s="9">
+      <c r="A10" s="4" t="n">
         <v>48470</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="4">
+      <c r="B10" s="5" t="inlineStr">
+        <is>
+          <t>"25:17"</t>
+        </is>
+      </c>
+      <c r="C10" s="5" t="inlineStr">
+        <is>
+          <t>Yeah, I feel I would actually like to see the 18-year term limits. I think when the lifetime limits were put in place way back in the 1800's life expectancy wasn't expected to be into the 80s and 90s like today and I don't really like the idea of having someone on the Supreme Court for 30 40, even 50 years, I also think would maybe take a little bit of the polarization out of it. If each president were to get to, you wouldn't have some of the games that are being played right now and it's kind of morbid. It feels like they're making current Supreme.</t>
+        </is>
+      </c>
+    </row>
+    <row r="11" ht="20" customHeight="1" s="9">
+      <c r="A11" s="4" t="n">
         <v>48470</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="4">
+      <c r="B11" s="5" t="inlineStr">
+        <is>
+          <t>"25:17"</t>
+        </is>
+      </c>
+      <c r="C11" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Or justices feel like they have to retire because they might die before a term ends, or after a term beds. So, I think this would kind of even things out a little bit better.</t>
+        </is>
+      </c>
+    </row>
+    <row r="12" ht="20" customHeight="1" s="9">
+      <c r="A12" s="4" t="n">
         <v>48508</v>
       </c>
-      <c r="B12" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="4">
+      <c r="B12" s="5" t="inlineStr">
+        <is>
+          <t>"26:04"</t>
+        </is>
+      </c>
+      <c r="C12" s="5" t="inlineStr">
+        <is>
+          <t>Why do we the founding fathers? Set it up. So these judges have tenure and they're Untouchable that have to worry about that and ethical decisions of the Supreme Court Justices. I think that self-regulating. I mean, we trust him enough to not do any unethical things. Obviously, that's coming up with Justice Thomas right now and giving each president,</t>
+        </is>
+      </c>
+    </row>
+    <row r="13" ht="20" customHeight="1" s="9">
+      <c r="A13" s="4" t="n">
         <v>48508</v>
       </c>
-      <c r="B13" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="4">
+      <c r="B13" s="5" t="inlineStr">
+        <is>
+          <t>"26:04"</t>
+        </is>
+      </c>
+      <c r="C13" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> it's, you know, just</t>
+        </is>
+      </c>
+    </row>
+    <row r="14" ht="20" customHeight="1" s="9">
+      <c r="A14" s="4" t="n">
         <v>48508</v>
       </c>
-      <c r="B14" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="4">
+      <c r="B14" s="5" t="inlineStr">
+        <is>
+          <t>"26:04"</t>
+        </is>
+      </c>
+      <c r="C14" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> the reason we're talking about this is because Trump was able to not put in three Supreme Court Justices, that's why this issues coming up and trying to</t>
+        </is>
+      </c>
+    </row>
+    <row r="15" ht="20" customHeight="1" s="9">
+      <c r="A15" s="4" t="n">
         <v>48508</v>
       </c>
-      <c r="B15" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C15" s="6"/>
-    </row>
-    <row r="16" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="4">
+      <c r="B15" s="5" t="inlineStr">
+        <is>
+          <t>"28:40"</t>
+        </is>
+      </c>
+      <c r="C15" s="6" t="n"/>
+    </row>
+    <row r="16" ht="20" customHeight="1" s="9">
+      <c r="A16" s="4" t="n">
         <v>48508</v>
       </c>
-      <c r="B16" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="4">
+      <c r="B16" s="5" t="inlineStr">
+        <is>
+          <t>"28:40"</t>
+        </is>
+      </c>
+      <c r="C16" s="5" t="inlineStr">
+        <is>
+          <t>Yes, I'll be for increasing federal spending on our public schools for how our government works. I'm working with a 19 year old man right now out of high school. Who does not know? There are three branches of government. So yeah, we can do more of that.</t>
+        </is>
+      </c>
+    </row>
+    <row r="17" ht="20" customHeight="1" s="9">
+      <c r="A17" s="4" t="n">
         <v>48470</v>
       </c>
-      <c r="B17" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="4">
+      <c r="B17" s="5" t="inlineStr">
+        <is>
+          <t>"29:05"</t>
+        </is>
+      </c>
+      <c r="C17" s="5" t="inlineStr">
+        <is>
+          <t>Yeah, I completely agree. I think it's not a bad thing as a father to two teenagers right now. I'm not expecting like Leaps and Bounds changes. I think it's things like financial literacy in. This is kind of a higher level topic for kids, but just to give them kind of that background and so that they can kind of have those basic understandings is never a bad thing. And I think we do a better job of just giving the kids, some type of introduction to government things like financial literacy, and things like that. Just so that they have kind of an idea of what it's all about.</t>
+        </is>
+      </c>
+    </row>
+    <row r="18" ht="20" customHeight="1" s="9">
+      <c r="A18" s="4" t="n">
         <v>48470</v>
       </c>
-      <c r="B18" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="4">
+      <c r="B18" s="5" t="inlineStr">
+        <is>
+          <t>"29:05"</t>
+        </is>
+      </c>
+      <c r="C18" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Out.</t>
+        </is>
+      </c>
+    </row>
+    <row r="19" ht="20" customHeight="1" s="9">
+      <c r="A19" s="4" t="n">
         <v>48508</v>
       </c>
-      <c r="B19" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="4">
+      <c r="B19" s="5" t="inlineStr">
+        <is>
+          <t>"33:27"</t>
+        </is>
+      </c>
+      <c r="C19" s="5" t="inlineStr">
+        <is>
+          <t>Germany is so real and it is fixed system. Maybe we could have it done by just geographical landmarks, instead like rivers and county lines instead of having. Just one street, the one district and another, the same exact story could be in another District. It's so weighted against the party in charge when they figure out.</t>
+        </is>
+      </c>
+    </row>
+    <row r="20" ht="20" customHeight="1" s="9">
+      <c r="A20" s="4" t="n">
         <v>48508</v>
       </c>
-      <c r="B20" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>29</v>
+      <c r="B20" s="5" t="inlineStr">
+        <is>
+          <t>"33:27"</t>
+        </is>
+      </c>
+      <c r="C20" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Out these lines.</t>
+        </is>
       </c>
     </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup orientation="portrait"/>
   <headerFooter>
-    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+    <oddHeader/>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12 &amp;K000000&amp;P</oddFooter>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
   </headerFooter>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EB3CAC0-E221-6740-B135-5AA3C7B15FEF}">
-  <dimension ref="A1:A14"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A1" s="7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" ht="15" x14ac:dyDescent="0.15">
-      <c r="A2" s="8" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" ht="15" x14ac:dyDescent="0.15">
-      <c r="A3" s="8" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" ht="15" x14ac:dyDescent="0.15">
-      <c r="A4" s="8" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" ht="15" x14ac:dyDescent="0.15">
-      <c r="A5" s="8" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" ht="15" x14ac:dyDescent="0.15">
-      <c r="A6" s="8" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" ht="15" x14ac:dyDescent="0.15">
-      <c r="A7" s="8" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" ht="15" x14ac:dyDescent="0.15">
-      <c r="A8" s="8" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" ht="15" x14ac:dyDescent="0.15">
-      <c r="A9" s="8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" ht="15" x14ac:dyDescent="0.15">
-      <c r="A10" s="8" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" ht="15" x14ac:dyDescent="0.15">
-      <c r="A11" s="8" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" ht="15" x14ac:dyDescent="0.15">
-      <c r="A12" s="8" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" ht="15" x14ac:dyDescent="0.15">
-      <c r="A13" s="8" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" ht="15" x14ac:dyDescent="0.15">
-      <c r="A14" s="8" t="s">
-        <v>45</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>